<commit_message>
added full isso service support
</commit_message>
<xml_diff>
--- a/testFile.xlsx
+++ b/testFile.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Код иссо</t>
   </si>
   <si>
+    <t>Тип иссо</t>
+  </si>
+  <si>
     <t>ФКУ</t>
   </si>
   <si>
@@ -26,28 +29,37 @@
     <t>Код дороги АБДМ</t>
   </si>
   <si>
+    <t>Id дорог АБДД</t>
+  </si>
+  <si>
     <t>КМ</t>
   </si>
   <si>
     <t>М</t>
   </si>
   <si>
-    <t>2300039</t>
-  </si>
-  <si>
-    <t>ФКУ "Центравтомагистраль"</t>
-  </si>
-  <si>
-    <t>"Московское большое кольцо" Дмитров - Сергиев Посад - Орехово-Зуево - Воскресенск - Михнево - Балабаново - Руза - Клин - Дмитров. Подъезд к государственному комплексу "Таруса" и проезды по его территории</t>
-  </si>
-  <si>
-    <t>6700</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>1100101</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>ФКУ Упрдор "Прибайкалье"</t>
+  </si>
+  <si>
+    <t>"Вилюй" Тулун - Братск - Усть-Кут - Мирный - Якутск</t>
+  </si>
+  <si>
+    <t>5030</t>
+  </si>
+  <si>
+    <t>56196a2d-5830-4b45-94e5-682d84e96aaf</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>518</t>
   </si>
 </sst>
 </file>
@@ -186,18 +198,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="true"/>
-    <col min="2" max="2" width="31.25" customWidth="true"/>
+    <col min="2" max="2" width="15.625" customWidth="true"/>
     <col min="3" max="3" width="31.25" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="4" max="4" width="31.25" customWidth="true"/>
+    <col min="5" max="5" width="27.34375" customWidth="true"/>
+    <col min="6" max="6" width="39.0625" customWidth="true"/>
+    <col min="7" max="7" width="15.625" customWidth="true"/>
+    <col min="8" max="8" width="15.625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -219,25 +233,37 @@
       <c r="F1" t="s" s="1">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>